<commit_message>
chapter 2 practice finished
</commit_message>
<xml_diff>
--- a/1999年某地区农户家庭经营性纯收入水平及其构成.xlsx
+++ b/1999年某地区农户家庭经营性纯收入水平及其构成.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1580\Desktop\课程文件\第二章 地理数据\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\professional\Quantitative Geography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DAD234-376B-46AA-A3B3-9BEAAD16BF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA81552-9FC6-4307-9794-55053F687BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4673" yWindow="1575" windowWidth="15622" windowHeight="11333" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$4:$E$13</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -198,16 +201,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -225,7 +225,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -511,12 +515,12 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,174 +530,302 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" ht="25.5" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1645.53</v>
+      </c>
+      <c r="E3">
+        <v>56.729111794475799</v>
+      </c>
+      <c r="F3">
+        <v>56.729111794475799</v>
+      </c>
+      <c r="G3">
+        <v>11.1111111111111</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3" s="10">
+        <v>763.62370202848899</v>
+      </c>
+      <c r="J3">
+        <v>500</v>
+      </c>
+      <c r="K3">
+        <v>900</v>
+      </c>
+      <c r="L3">
+        <v>0.65905925507122398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="3"/>
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="9">
-        <v>1645.53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="8">
+        <v>390.24</v>
+      </c>
+      <c r="E4">
+        <v>13.453397134465</v>
+      </c>
+      <c r="F4">
+        <v>70.182508928940806</v>
+      </c>
+      <c r="G4">
+        <v>22.2222222222222</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="8">
+        <v>211.62</v>
+      </c>
+      <c r="E5">
+        <v>7.2955307031454701</v>
+      </c>
+      <c r="F5">
+        <v>77.478039632086293</v>
+      </c>
+      <c r="G5">
+        <v>33.3333333333333</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8">
+        <v>167.38</v>
+      </c>
+      <c r="E6">
+        <v>5.7703710854006598</v>
+      </c>
+      <c r="F6">
+        <v>83.248410717486905</v>
+      </c>
+      <c r="G6">
+        <v>44.4444444444444</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" s="3"/>
+      <c r="B7" s="6">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="8">
+        <v>150.88</v>
+      </c>
+      <c r="E7">
+        <v>5.20153894948771</v>
+      </c>
+      <c r="F7">
+        <v>88.449949666974703</v>
+      </c>
+      <c r="G7">
+        <v>55.5555555555556</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A8" s="3"/>
+      <c r="B8" s="6">
+        <v>9</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8">
+        <v>136.69999999999999</v>
+      </c>
+      <c r="E8">
+        <v>4.7126880593516001</v>
+      </c>
+      <c r="F8">
+        <v>93.162637726326196</v>
+      </c>
+      <c r="G8">
+        <v>66.6666666666667</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D9" s="8">
         <v>79.66</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="7">
-        <v>3</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="9">
-        <v>390.24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="7">
+      <c r="E9">
+        <v>2.7462526028379601</v>
+      </c>
+      <c r="F9">
+        <v>95.908890329164194</v>
+      </c>
+      <c r="G9">
+        <v>77.7777777777778</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A10" s="3"/>
+      <c r="B10" s="6">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D10" s="8">
         <v>74.12</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="7">
-        <v>5</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="9">
-        <v>167.38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="7">
+      <c r="E10">
+        <v>2.5552629038708199</v>
+      </c>
+      <c r="F10">
+        <v>98.464153233035006</v>
+      </c>
+      <c r="G10">
+        <v>88.8888888888889</v>
+      </c>
+      <c r="H10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A11" s="3"/>
+      <c r="B11" s="6">
         <v>6</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D11" s="8">
         <v>44.55</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="7">
-        <v>7</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="9">
-        <v>150.88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="7">
-        <v>8</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="9">
-        <v>211.62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>1.53584676696499</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
-      <c r="B12" s="7">
-        <v>9</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="9">
-        <v>136.69999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="11">
+        <v>2900.68</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
-      <c r="B13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="10"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H12">
+    <sortCondition descending="1" ref="E2:E12"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="I1:L1"/>
   </mergeCells>

</xml_diff>